<commit_message>
Add new item ''Line' in turnover items
</commit_message>
<xml_diff>
--- a/basketBallRecorder/PPP數據.xlsx
+++ b/basketBallRecorder/PPP數據.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27021"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="全隊" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="59">
   <si>
     <t>快攻(F)</t>
   </si>
@@ -245,6 +245,10 @@
   </si>
   <si>
     <t>犯規()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Line</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -430,14 +434,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -451,6 +461,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -463,12 +497,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -487,31 +515,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="9" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -840,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GV3"/>
+  <dimension ref="A1:GW3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="EE1" workbookViewId="0">
+      <selection activeCell="EU10" sqref="EU10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -852,561 +871,563 @@
     <col min="2" max="204" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:204">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="1:205">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="18" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
       <c r="AB1" s="1"/>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="10" t="s">
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="10"/>
-      <c r="AZ1" s="10"/>
-      <c r="BA1" s="10"/>
-      <c r="BB1" s="10"/>
-      <c r="BC1" s="20" t="s">
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7"/>
+      <c r="AS1" s="7"/>
+      <c r="AT1" s="7"/>
+      <c r="AU1" s="7"/>
+      <c r="AV1" s="7"/>
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7"/>
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="BD1" s="20"/>
-      <c r="BE1" s="20"/>
-      <c r="BF1" s="20"/>
-      <c r="BG1" s="20"/>
-      <c r="BH1" s="20"/>
-      <c r="BI1" s="20"/>
-      <c r="BJ1" s="20"/>
-      <c r="BK1" s="20"/>
-      <c r="BL1" s="20"/>
-      <c r="BM1" s="20"/>
-      <c r="BN1" s="20"/>
-      <c r="BO1" s="20"/>
-      <c r="BP1" s="10" t="s">
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12"/>
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="BQ1" s="10"/>
-      <c r="BR1" s="10"/>
-      <c r="BS1" s="10"/>
-      <c r="BT1" s="10"/>
-      <c r="BU1" s="10"/>
-      <c r="BV1" s="10"/>
-      <c r="BW1" s="10"/>
-      <c r="BX1" s="10"/>
-      <c r="BY1" s="10"/>
-      <c r="BZ1" s="10"/>
-      <c r="CA1" s="10"/>
-      <c r="CB1" s="10"/>
-      <c r="CC1" s="9" t="s">
+      <c r="BQ1" s="7"/>
+      <c r="BR1" s="7"/>
+      <c r="BS1" s="7"/>
+      <c r="BT1" s="7"/>
+      <c r="BU1" s="7"/>
+      <c r="BV1" s="7"/>
+      <c r="BW1" s="7"/>
+      <c r="BX1" s="7"/>
+      <c r="BY1" s="7"/>
+      <c r="BZ1" s="7"/>
+      <c r="CA1" s="7"/>
+      <c r="CB1" s="7"/>
+      <c r="CC1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="CD1" s="9"/>
-      <c r="CE1" s="9"/>
-      <c r="CF1" s="9"/>
-      <c r="CG1" s="9"/>
-      <c r="CH1" s="9"/>
-      <c r="CI1" s="9"/>
-      <c r="CJ1" s="9"/>
-      <c r="CK1" s="9"/>
-      <c r="CL1" s="9"/>
-      <c r="CM1" s="9"/>
-      <c r="CN1" s="9"/>
-      <c r="CO1" s="9"/>
-      <c r="CP1" s="9"/>
-      <c r="CQ1" s="9"/>
-      <c r="CR1" s="9"/>
-      <c r="CS1" s="9"/>
-      <c r="CT1" s="9"/>
-      <c r="CU1" s="9"/>
-      <c r="CV1" s="9"/>
-      <c r="CW1" s="9"/>
-      <c r="CX1" s="9"/>
-      <c r="CY1" s="9"/>
-      <c r="CZ1" s="9"/>
-      <c r="DA1" s="9"/>
-      <c r="DB1" s="10" t="s">
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="8"/>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8"/>
+      <c r="CV1" s="8"/>
+      <c r="CW1" s="8"/>
+      <c r="CX1" s="8"/>
+      <c r="CY1" s="8"/>
+      <c r="CZ1" s="8"/>
+      <c r="DA1" s="8"/>
+      <c r="DB1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="DC1" s="10"/>
-      <c r="DD1" s="10"/>
-      <c r="DE1" s="10"/>
-      <c r="DF1" s="10"/>
-      <c r="DG1" s="10"/>
-      <c r="DH1" s="10"/>
-      <c r="DI1" s="10"/>
-      <c r="DJ1" s="10"/>
-      <c r="DK1" s="10"/>
-      <c r="DL1" s="10"/>
-      <c r="DM1" s="10"/>
-      <c r="DN1" s="10"/>
-      <c r="DO1" s="10"/>
-      <c r="DP1" s="10"/>
-      <c r="DQ1" s="10"/>
-      <c r="DR1" s="10"/>
-      <c r="DS1" s="9" t="s">
+      <c r="DC1" s="7"/>
+      <c r="DD1" s="7"/>
+      <c r="DE1" s="7"/>
+      <c r="DF1" s="7"/>
+      <c r="DG1" s="7"/>
+      <c r="DH1" s="7"/>
+      <c r="DI1" s="7"/>
+      <c r="DJ1" s="7"/>
+      <c r="DK1" s="7"/>
+      <c r="DL1" s="7"/>
+      <c r="DM1" s="7"/>
+      <c r="DN1" s="7"/>
+      <c r="DO1" s="7"/>
+      <c r="DP1" s="7"/>
+      <c r="DQ1" s="7"/>
+      <c r="DR1" s="7"/>
+      <c r="DS1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="DT1" s="9"/>
-      <c r="DU1" s="9"/>
-      <c r="DV1" s="9"/>
-      <c r="DW1" s="9"/>
-      <c r="DX1" s="9"/>
-      <c r="DY1" s="9"/>
-      <c r="DZ1" s="9"/>
-      <c r="EA1" s="9"/>
-      <c r="EB1" s="9"/>
-      <c r="EC1" s="9"/>
-      <c r="ED1" s="9"/>
-      <c r="EE1" s="9"/>
-      <c r="EF1" s="9"/>
-      <c r="EG1" s="9"/>
-      <c r="EH1" s="9"/>
-      <c r="EI1" s="9"/>
-      <c r="EJ1" s="9"/>
-      <c r="EK1" s="9"/>
-      <c r="EL1" s="9"/>
-      <c r="EM1" s="9"/>
-      <c r="EN1" s="11" t="s">
+      <c r="DT1" s="8"/>
+      <c r="DU1" s="8"/>
+      <c r="DV1" s="8"/>
+      <c r="DW1" s="8"/>
+      <c r="DX1" s="8"/>
+      <c r="DY1" s="8"/>
+      <c r="DZ1" s="8"/>
+      <c r="EA1" s="8"/>
+      <c r="EB1" s="8"/>
+      <c r="EC1" s="8"/>
+      <c r="ED1" s="8"/>
+      <c r="EE1" s="8"/>
+      <c r="EF1" s="8"/>
+      <c r="EG1" s="8"/>
+      <c r="EH1" s="8"/>
+      <c r="EI1" s="8"/>
+      <c r="EJ1" s="8"/>
+      <c r="EK1" s="8"/>
+      <c r="EL1" s="8"/>
+      <c r="EM1" s="8"/>
+      <c r="EN1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="EO1" s="12"/>
-      <c r="EP1" s="12"/>
-      <c r="EQ1" s="12"/>
-      <c r="ER1" s="12"/>
-      <c r="ES1" s="12"/>
-      <c r="ET1" s="13"/>
-      <c r="EU1" s="9" t="s">
+      <c r="EO1" s="18"/>
+      <c r="EP1" s="18"/>
+      <c r="EQ1" s="18"/>
+      <c r="ER1" s="18"/>
+      <c r="ES1" s="18"/>
+      <c r="ET1" s="18"/>
+      <c r="EU1" s="19"/>
+      <c r="EV1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="EV1" s="9"/>
-      <c r="EW1" s="9"/>
-      <c r="EX1" s="9"/>
-      <c r="EY1" s="9"/>
-      <c r="EZ1" s="9"/>
-      <c r="FA1" s="9"/>
-      <c r="FB1" s="9"/>
-      <c r="FC1" s="9"/>
-      <c r="FD1" s="9"/>
-      <c r="FE1" s="9"/>
-      <c r="FF1" s="9"/>
-      <c r="FG1" s="9"/>
-      <c r="FH1" s="9"/>
-      <c r="FI1" s="9"/>
-      <c r="FJ1" s="9"/>
-      <c r="FK1" s="9"/>
-      <c r="FL1" s="9"/>
-      <c r="FM1" s="9"/>
-      <c r="FN1" s="9"/>
-      <c r="FO1" s="9"/>
-      <c r="FP1" s="9"/>
-      <c r="FQ1" s="9"/>
-      <c r="FR1" s="9"/>
-      <c r="FS1" s="9"/>
-      <c r="FT1" s="9"/>
-      <c r="FU1" s="9"/>
-      <c r="FV1" s="9"/>
-      <c r="FW1" s="9"/>
-      <c r="FX1" s="9"/>
-      <c r="FY1" s="9"/>
-      <c r="FZ1" s="9"/>
-      <c r="GA1" s="9"/>
-      <c r="GB1" s="9"/>
-      <c r="GC1" s="9"/>
-      <c r="GD1" s="9"/>
-      <c r="GE1" s="9"/>
-      <c r="GF1" s="9"/>
-      <c r="GG1" s="9"/>
-      <c r="GH1" s="9"/>
-      <c r="GI1" s="9"/>
-      <c r="GJ1" s="9"/>
-      <c r="GK1" s="9"/>
-      <c r="GL1" s="9"/>
-      <c r="GM1" s="9"/>
-      <c r="GN1" s="9"/>
-      <c r="GO1" s="9"/>
-      <c r="GP1" s="9"/>
-      <c r="GQ1" s="9"/>
-      <c r="GR1" s="9"/>
-      <c r="GS1" s="9"/>
-      <c r="GT1" s="9"/>
-      <c r="GU1" s="9"/>
-      <c r="GV1" s="9"/>
+      <c r="EW1" s="8"/>
+      <c r="EX1" s="8"/>
+      <c r="EY1" s="8"/>
+      <c r="EZ1" s="8"/>
+      <c r="FA1" s="8"/>
+      <c r="FB1" s="8"/>
+      <c r="FC1" s="8"/>
+      <c r="FD1" s="8"/>
+      <c r="FE1" s="8"/>
+      <c r="FF1" s="8"/>
+      <c r="FG1" s="8"/>
+      <c r="FH1" s="8"/>
+      <c r="FI1" s="8"/>
+      <c r="FJ1" s="8"/>
+      <c r="FK1" s="8"/>
+      <c r="FL1" s="8"/>
+      <c r="FM1" s="8"/>
+      <c r="FN1" s="8"/>
+      <c r="FO1" s="8"/>
+      <c r="FP1" s="8"/>
+      <c r="FQ1" s="8"/>
+      <c r="FR1" s="8"/>
+      <c r="FS1" s="8"/>
+      <c r="FT1" s="8"/>
+      <c r="FU1" s="8"/>
+      <c r="FV1" s="8"/>
+      <c r="FW1" s="8"/>
+      <c r="FX1" s="8"/>
+      <c r="FY1" s="8"/>
+      <c r="FZ1" s="8"/>
+      <c r="GA1" s="8"/>
+      <c r="GB1" s="8"/>
+      <c r="GC1" s="8"/>
+      <c r="GD1" s="8"/>
+      <c r="GE1" s="8"/>
+      <c r="GF1" s="8"/>
+      <c r="GG1" s="8"/>
+      <c r="GH1" s="8"/>
+      <c r="GI1" s="8"/>
+      <c r="GJ1" s="8"/>
+      <c r="GK1" s="8"/>
+      <c r="GL1" s="8"/>
+      <c r="GM1" s="8"/>
+      <c r="GN1" s="8"/>
+      <c r="GO1" s="8"/>
+      <c r="GP1" s="8"/>
+      <c r="GQ1" s="8"/>
+      <c r="GR1" s="8"/>
+      <c r="GS1" s="8"/>
+      <c r="GT1" s="8"/>
+      <c r="GU1" s="8"/>
+      <c r="GV1" s="8"/>
+      <c r="GW1" s="8"/>
     </row>
-    <row r="2" spans="1:204">
+    <row r="2" spans="1:205">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
       <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="6" t="s">
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="6" t="s">
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="8"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="16"/>
       <c r="AB2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AC2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5" t="s">
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5" t="s">
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
       <c r="AO2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AP2" s="5" t="s">
+      <c r="AP2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5" t="s">
+      <c r="AQ2" s="13"/>
+      <c r="AR2" s="13"/>
+      <c r="AS2" s="13"/>
+      <c r="AT2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5"/>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5" t="s">
+      <c r="AU2" s="13"/>
+      <c r="AV2" s="13"/>
+      <c r="AW2" s="13"/>
+      <c r="AX2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="5"/>
+      <c r="AY2" s="13"/>
+      <c r="AZ2" s="13"/>
+      <c r="BA2" s="13"/>
       <c r="BB2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="BC2" s="5" t="s">
+      <c r="BC2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5"/>
-      <c r="BG2" s="5" t="s">
+      <c r="BD2" s="13"/>
+      <c r="BE2" s="13"/>
+      <c r="BF2" s="13"/>
+      <c r="BG2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5"/>
-      <c r="BJ2" s="5"/>
-      <c r="BK2" s="5" t="s">
+      <c r="BH2" s="13"/>
+      <c r="BI2" s="13"/>
+      <c r="BJ2" s="13"/>
+      <c r="BK2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="BL2" s="5"/>
-      <c r="BM2" s="5"/>
-      <c r="BN2" s="5"/>
+      <c r="BL2" s="13"/>
+      <c r="BM2" s="13"/>
+      <c r="BN2" s="13"/>
       <c r="BO2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BP2" s="5" t="s">
+      <c r="BP2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="BQ2" s="5"/>
-      <c r="BR2" s="5"/>
-      <c r="BS2" s="5"/>
-      <c r="BT2" s="5" t="s">
+      <c r="BQ2" s="13"/>
+      <c r="BR2" s="13"/>
+      <c r="BS2" s="13"/>
+      <c r="BT2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="BU2" s="5"/>
-      <c r="BV2" s="5"/>
-      <c r="BW2" s="5"/>
-      <c r="BX2" s="5" t="s">
+      <c r="BU2" s="13"/>
+      <c r="BV2" s="13"/>
+      <c r="BW2" s="13"/>
+      <c r="BX2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="BY2" s="5"/>
-      <c r="BZ2" s="5"/>
-      <c r="CA2" s="5"/>
+      <c r="BY2" s="13"/>
+      <c r="BZ2" s="13"/>
+      <c r="CA2" s="13"/>
       <c r="CB2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="CC2" s="5" t="s">
+      <c r="CC2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="CD2" s="5"/>
-      <c r="CE2" s="5"/>
-      <c r="CF2" s="5"/>
-      <c r="CG2" s="5" t="s">
+      <c r="CD2" s="13"/>
+      <c r="CE2" s="13"/>
+      <c r="CF2" s="13"/>
+      <c r="CG2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="CH2" s="5"/>
-      <c r="CI2" s="5"/>
-      <c r="CJ2" s="5"/>
-      <c r="CK2" s="5" t="s">
+      <c r="CH2" s="13"/>
+      <c r="CI2" s="13"/>
+      <c r="CJ2" s="13"/>
+      <c r="CK2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="CL2" s="5"/>
-      <c r="CM2" s="5"/>
-      <c r="CN2" s="5"/>
-      <c r="CO2" s="5" t="s">
+      <c r="CL2" s="13"/>
+      <c r="CM2" s="13"/>
+      <c r="CN2" s="13"/>
+      <c r="CO2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="CP2" s="5"/>
-      <c r="CQ2" s="5"/>
-      <c r="CR2" s="5"/>
-      <c r="CS2" s="5" t="s">
+      <c r="CP2" s="13"/>
+      <c r="CQ2" s="13"/>
+      <c r="CR2" s="13"/>
+      <c r="CS2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="CT2" s="5"/>
-      <c r="CU2" s="5"/>
-      <c r="CV2" s="5"/>
-      <c r="CW2" s="5" t="s">
+      <c r="CT2" s="13"/>
+      <c r="CU2" s="13"/>
+      <c r="CV2" s="13"/>
+      <c r="CW2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="CX2" s="5"/>
-      <c r="CY2" s="5"/>
-      <c r="CZ2" s="5"/>
+      <c r="CX2" s="13"/>
+      <c r="CY2" s="13"/>
+      <c r="CZ2" s="13"/>
       <c r="DA2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="DB2" s="5" t="s">
+      <c r="DB2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="DC2" s="5"/>
-      <c r="DD2" s="5"/>
-      <c r="DE2" s="5"/>
-      <c r="DF2" s="5" t="s">
+      <c r="DC2" s="13"/>
+      <c r="DD2" s="13"/>
+      <c r="DE2" s="13"/>
+      <c r="DF2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="DG2" s="5"/>
-      <c r="DH2" s="5"/>
-      <c r="DI2" s="5"/>
-      <c r="DJ2" s="5" t="s">
+      <c r="DG2" s="13"/>
+      <c r="DH2" s="13"/>
+      <c r="DI2" s="13"/>
+      <c r="DJ2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="DK2" s="5"/>
-      <c r="DL2" s="5"/>
-      <c r="DM2" s="5"/>
-      <c r="DN2" s="5" t="s">
+      <c r="DK2" s="13"/>
+      <c r="DL2" s="13"/>
+      <c r="DM2" s="13"/>
+      <c r="DN2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="DO2" s="5"/>
-      <c r="DP2" s="5"/>
-      <c r="DQ2" s="5"/>
+      <c r="DO2" s="13"/>
+      <c r="DP2" s="13"/>
+      <c r="DQ2" s="13"/>
       <c r="DR2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="DS2" s="5" t="s">
+      <c r="DS2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="DT2" s="5"/>
-      <c r="DU2" s="5"/>
-      <c r="DV2" s="5"/>
-      <c r="DW2" s="5" t="s">
+      <c r="DT2" s="13"/>
+      <c r="DU2" s="13"/>
+      <c r="DV2" s="13"/>
+      <c r="DW2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="DX2" s="5"/>
-      <c r="DY2" s="5"/>
-      <c r="DZ2" s="5"/>
-      <c r="EA2" s="5" t="s">
+      <c r="DX2" s="13"/>
+      <c r="DY2" s="13"/>
+      <c r="DZ2" s="13"/>
+      <c r="EA2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="EB2" s="5"/>
-      <c r="EC2" s="5"/>
-      <c r="ED2" s="5"/>
-      <c r="EE2" s="5" t="s">
+      <c r="EB2" s="13"/>
+      <c r="EC2" s="13"/>
+      <c r="ED2" s="13"/>
+      <c r="EE2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="EF2" s="5"/>
-      <c r="EG2" s="5"/>
-      <c r="EH2" s="5"/>
-      <c r="EI2" s="5" t="s">
+      <c r="EF2" s="13"/>
+      <c r="EG2" s="13"/>
+      <c r="EH2" s="13"/>
+      <c r="EI2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="EJ2" s="5"/>
-      <c r="EK2" s="5"/>
-      <c r="EL2" s="5"/>
+      <c r="EJ2" s="13"/>
+      <c r="EK2" s="13"/>
+      <c r="EL2" s="13"/>
       <c r="EM2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="EN2" s="14"/>
-      <c r="EO2" s="15"/>
-      <c r="EP2" s="15"/>
-      <c r="EQ2" s="15"/>
-      <c r="ER2" s="15"/>
-      <c r="ES2" s="15"/>
-      <c r="ET2" s="16"/>
-      <c r="EU2" s="5" t="s">
+      <c r="EN2" s="20"/>
+      <c r="EO2" s="21"/>
+      <c r="EP2" s="21"/>
+      <c r="EQ2" s="21"/>
+      <c r="ER2" s="21"/>
+      <c r="ES2" s="21"/>
+      <c r="ET2" s="21"/>
+      <c r="EU2" s="22"/>
+      <c r="EV2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="EV2" s="5"/>
-      <c r="EW2" s="5"/>
-      <c r="EX2" s="5"/>
-      <c r="EY2" s="5" t="s">
+      <c r="EW2" s="13"/>
+      <c r="EX2" s="13"/>
+      <c r="EY2" s="13"/>
+      <c r="EZ2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="EZ2" s="5"/>
-      <c r="FA2" s="5"/>
-      <c r="FB2" s="5"/>
-      <c r="FC2" s="5" t="s">
+      <c r="FA2" s="13"/>
+      <c r="FB2" s="13"/>
+      <c r="FC2" s="13"/>
+      <c r="FD2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="FD2" s="5"/>
-      <c r="FE2" s="5"/>
-      <c r="FF2" s="5"/>
-      <c r="FG2" s="5" t="s">
+      <c r="FE2" s="13"/>
+      <c r="FF2" s="13"/>
+      <c r="FG2" s="13"/>
+      <c r="FH2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="FH2" s="5"/>
-      <c r="FI2" s="5"/>
-      <c r="FJ2" s="5"/>
-      <c r="FK2" s="5" t="s">
+      <c r="FI2" s="13"/>
+      <c r="FJ2" s="13"/>
+      <c r="FK2" s="13"/>
+      <c r="FL2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="FL2" s="5"/>
-      <c r="FM2" s="5"/>
-      <c r="FN2" s="5"/>
-      <c r="FO2" s="5" t="s">
+      <c r="FM2" s="13"/>
+      <c r="FN2" s="13"/>
+      <c r="FO2" s="13"/>
+      <c r="FP2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="FP2" s="5"/>
-      <c r="FQ2" s="5"/>
-      <c r="FR2" s="5"/>
-      <c r="FS2" s="5" t="s">
+      <c r="FQ2" s="13"/>
+      <c r="FR2" s="13"/>
+      <c r="FS2" s="13"/>
+      <c r="FT2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="FT2" s="5"/>
-      <c r="FU2" s="5"/>
-      <c r="FV2" s="5"/>
-      <c r="FW2" s="5" t="s">
+      <c r="FU2" s="13"/>
+      <c r="FV2" s="13"/>
+      <c r="FW2" s="13"/>
+      <c r="FX2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="FX2" s="5"/>
-      <c r="FY2" s="5"/>
-      <c r="FZ2" s="5"/>
-      <c r="GA2" s="5" t="s">
+      <c r="FY2" s="13"/>
+      <c r="FZ2" s="13"/>
+      <c r="GA2" s="13"/>
+      <c r="GB2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="GB2" s="5"/>
-      <c r="GC2" s="5"/>
-      <c r="GD2" s="5"/>
-      <c r="GE2" s="5" t="s">
+      <c r="GC2" s="13"/>
+      <c r="GD2" s="13"/>
+      <c r="GE2" s="13"/>
+      <c r="GF2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="GF2" s="5"/>
-      <c r="GG2" s="5"/>
-      <c r="GH2" s="5"/>
-      <c r="GI2" s="5" t="s">
+      <c r="GG2" s="13"/>
+      <c r="GH2" s="13"/>
+      <c r="GI2" s="13"/>
+      <c r="GJ2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="GJ2" s="5"/>
-      <c r="GK2" s="5"/>
-      <c r="GL2" s="5"/>
-      <c r="GM2" s="5" t="s">
+      <c r="GK2" s="13"/>
+      <c r="GL2" s="13"/>
+      <c r="GM2" s="13"/>
+      <c r="GN2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="GN2" s="5"/>
-      <c r="GO2" s="5"/>
-      <c r="GP2" s="5"/>
-      <c r="GQ2" s="5" t="s">
+      <c r="GO2" s="13"/>
+      <c r="GP2" s="13"/>
+      <c r="GQ2" s="13"/>
+      <c r="GR2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="GR2" s="5" t="s">
+      <c r="GS2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="GS2" s="5" t="s">
+      <c r="GT2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="GT2" s="5" t="s">
+      <c r="GU2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="GU2" s="5" t="s">
+      <c r="GV2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="GV2" s="5" t="s">
+      <c r="GW2" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:204">
+    <row r="3" spans="1:205">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -1848,184 +1869,195 @@
       <c r="EQ3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="ER3" s="2" t="s">
+      <c r="ER3" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="ES3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="ES3" s="2" t="s">
+      <c r="ET3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="ET3" s="2" t="s">
+      <c r="EU3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="EU3" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="EV3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="EW3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="EX3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="EY3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="EZ3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="FA3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="FB3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="FC3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="FD3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="FE3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="FF3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="FG3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="FH3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="FI3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="FJ3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="FK3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="FL3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="FM3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="FN3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="FO3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="FP3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="FQ3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="FR3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="FS3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="FT3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="FU3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="FV3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="FW3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="FX3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="FY3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="FZ3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="GA3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="GB3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="GC3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="GD3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="GE3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="GF3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="GG3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="GH3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="GI3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="GJ3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="GK3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="GL3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="GM3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="GN3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="GO3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="GP3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="GQ3" s="5"/>
-      <c r="GR3" s="5"/>
-      <c r="GS3" s="5"/>
-      <c r="GT3" s="5"/>
-      <c r="GU3" s="5"/>
-      <c r="GV3" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="GQ3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="GR3" s="13"/>
+      <c r="GS3" s="13"/>
+      <c r="GT3" s="13"/>
+      <c r="GU3" s="13"/>
+      <c r="GV3" s="13"/>
+      <c r="GW3" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="BP1:CB1"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AA1"/>
-    <mergeCell ref="AC1:AO1"/>
-    <mergeCell ref="AP1:BB1"/>
-    <mergeCell ref="BC1:BO1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="CC1:DA1"/>
-    <mergeCell ref="DB1:DR1"/>
-    <mergeCell ref="DS1:EM1"/>
-    <mergeCell ref="EN1:ET2"/>
-    <mergeCell ref="EU1:GV1"/>
+    <mergeCell ref="GV2:GV3"/>
+    <mergeCell ref="GW2:GW3"/>
+    <mergeCell ref="GB2:GE2"/>
+    <mergeCell ref="GF2:GI2"/>
+    <mergeCell ref="GJ2:GM2"/>
+    <mergeCell ref="GN2:GQ2"/>
+    <mergeCell ref="GR2:GR3"/>
+    <mergeCell ref="GS2:GS3"/>
+    <mergeCell ref="FL2:FO2"/>
+    <mergeCell ref="FP2:FS2"/>
+    <mergeCell ref="FT2:FW2"/>
+    <mergeCell ref="GT2:GT3"/>
+    <mergeCell ref="GU2:GU3"/>
+    <mergeCell ref="EI2:EL2"/>
+    <mergeCell ref="EV2:EY2"/>
+    <mergeCell ref="EZ2:FC2"/>
+    <mergeCell ref="FD2:FG2"/>
+    <mergeCell ref="FH2:FK2"/>
+    <mergeCell ref="EN1:EU2"/>
+    <mergeCell ref="BX2:CA2"/>
+    <mergeCell ref="CC2:CF2"/>
+    <mergeCell ref="CG2:CJ2"/>
+    <mergeCell ref="CK2:CN2"/>
+    <mergeCell ref="CO2:CR2"/>
     <mergeCell ref="BT2:BW2"/>
     <mergeCell ref="X2:AA2"/>
     <mergeCell ref="AC2:AF2"/>
@@ -2038,40 +2070,32 @@
     <mergeCell ref="BG2:BJ2"/>
     <mergeCell ref="BK2:BN2"/>
     <mergeCell ref="BP2:BS2"/>
+    <mergeCell ref="CC1:DA1"/>
+    <mergeCell ref="DB1:DR1"/>
+    <mergeCell ref="DS1:EM1"/>
+    <mergeCell ref="EV1:GW1"/>
     <mergeCell ref="DS2:DV2"/>
-    <mergeCell ref="BX2:CA2"/>
-    <mergeCell ref="CC2:CF2"/>
-    <mergeCell ref="CG2:CJ2"/>
-    <mergeCell ref="CK2:CN2"/>
-    <mergeCell ref="CO2:CR2"/>
     <mergeCell ref="CS2:CV2"/>
     <mergeCell ref="CW2:CZ2"/>
     <mergeCell ref="DB2:DE2"/>
     <mergeCell ref="DF2:DI2"/>
     <mergeCell ref="DJ2:DM2"/>
     <mergeCell ref="DN2:DQ2"/>
-    <mergeCell ref="FW2:FZ2"/>
+    <mergeCell ref="FX2:GA2"/>
     <mergeCell ref="DW2:DZ2"/>
     <mergeCell ref="EA2:ED2"/>
     <mergeCell ref="EE2:EH2"/>
-    <mergeCell ref="EI2:EL2"/>
-    <mergeCell ref="EU2:EX2"/>
-    <mergeCell ref="EY2:FB2"/>
-    <mergeCell ref="FC2:FF2"/>
-    <mergeCell ref="FG2:FJ2"/>
-    <mergeCell ref="FK2:FN2"/>
-    <mergeCell ref="FO2:FR2"/>
-    <mergeCell ref="FS2:FV2"/>
-    <mergeCell ref="GS2:GS3"/>
-    <mergeCell ref="GT2:GT3"/>
-    <mergeCell ref="GU2:GU3"/>
-    <mergeCell ref="GV2:GV3"/>
-    <mergeCell ref="GA2:GD2"/>
-    <mergeCell ref="GE2:GH2"/>
-    <mergeCell ref="GI2:GL2"/>
-    <mergeCell ref="GM2:GP2"/>
-    <mergeCell ref="GQ2:GQ3"/>
-    <mergeCell ref="GR2:GR3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="BP1:CB1"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="AC1:AO1"/>
+    <mergeCell ref="AP1:BB1"/>
+    <mergeCell ref="BC1:BO1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Debug: Modify the text error in PPP xlsx
</commit_message>
<xml_diff>
--- a/basketBallRecorder/PPP數據.xlsx
+++ b/basketBallRecorder/PPP數據.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
   <si>
     <t>快攻(F)</t>
   </si>
@@ -244,11 +244,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>犯規()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>犯規(F)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出手(A)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -467,12 +471,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -483,39 +520,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -861,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GW3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EE1" workbookViewId="0">
-      <selection activeCell="EU10" sqref="EU10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -874,556 +878,556 @@
     <row r="1" spans="1:205">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="10" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
       <c r="AB1" s="1"/>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="7" t="s">
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7"/>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
-      <c r="BC1" s="12" t="s">
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="7" t="s">
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23"/>
+      <c r="BG1" s="23"/>
+      <c r="BH1" s="23"/>
+      <c r="BI1" s="23"/>
+      <c r="BJ1" s="23"/>
+      <c r="BK1" s="23"/>
+      <c r="BL1" s="23"/>
+      <c r="BM1" s="23"/>
+      <c r="BN1" s="23"/>
+      <c r="BO1" s="23"/>
+      <c r="BP1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BQ1" s="7"/>
-      <c r="BR1" s="7"/>
-      <c r="BS1" s="7"/>
-      <c r="BT1" s="7"/>
-      <c r="BU1" s="7"/>
-      <c r="BV1" s="7"/>
-      <c r="BW1" s="7"/>
-      <c r="BX1" s="7"/>
-      <c r="BY1" s="7"/>
-      <c r="BZ1" s="7"/>
-      <c r="CA1" s="7"/>
-      <c r="CB1" s="7"/>
-      <c r="CC1" s="8" t="s">
+      <c r="BQ1" s="19"/>
+      <c r="BR1" s="19"/>
+      <c r="BS1" s="19"/>
+      <c r="BT1" s="19"/>
+      <c r="BU1" s="19"/>
+      <c r="BV1" s="19"/>
+      <c r="BW1" s="19"/>
+      <c r="BX1" s="19"/>
+      <c r="BY1" s="19"/>
+      <c r="BZ1" s="19"/>
+      <c r="CA1" s="19"/>
+      <c r="CB1" s="19"/>
+      <c r="CC1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="CD1" s="8"/>
-      <c r="CE1" s="8"/>
-      <c r="CF1" s="8"/>
-      <c r="CG1" s="8"/>
-      <c r="CH1" s="8"/>
-      <c r="CI1" s="8"/>
-      <c r="CJ1" s="8"/>
-      <c r="CK1" s="8"/>
-      <c r="CL1" s="8"/>
-      <c r="CM1" s="8"/>
-      <c r="CN1" s="8"/>
-      <c r="CO1" s="8"/>
-      <c r="CP1" s="8"/>
-      <c r="CQ1" s="8"/>
-      <c r="CR1" s="8"/>
-      <c r="CS1" s="8"/>
-      <c r="CT1" s="8"/>
-      <c r="CU1" s="8"/>
-      <c r="CV1" s="8"/>
-      <c r="CW1" s="8"/>
-      <c r="CX1" s="8"/>
-      <c r="CY1" s="8"/>
-      <c r="CZ1" s="8"/>
-      <c r="DA1" s="8"/>
-      <c r="DB1" s="7" t="s">
+      <c r="CD1" s="18"/>
+      <c r="CE1" s="18"/>
+      <c r="CF1" s="18"/>
+      <c r="CG1" s="18"/>
+      <c r="CH1" s="18"/>
+      <c r="CI1" s="18"/>
+      <c r="CJ1" s="18"/>
+      <c r="CK1" s="18"/>
+      <c r="CL1" s="18"/>
+      <c r="CM1" s="18"/>
+      <c r="CN1" s="18"/>
+      <c r="CO1" s="18"/>
+      <c r="CP1" s="18"/>
+      <c r="CQ1" s="18"/>
+      <c r="CR1" s="18"/>
+      <c r="CS1" s="18"/>
+      <c r="CT1" s="18"/>
+      <c r="CU1" s="18"/>
+      <c r="CV1" s="18"/>
+      <c r="CW1" s="18"/>
+      <c r="CX1" s="18"/>
+      <c r="CY1" s="18"/>
+      <c r="CZ1" s="18"/>
+      <c r="DA1" s="18"/>
+      <c r="DB1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="DC1" s="7"/>
-      <c r="DD1" s="7"/>
-      <c r="DE1" s="7"/>
-      <c r="DF1" s="7"/>
-      <c r="DG1" s="7"/>
-      <c r="DH1" s="7"/>
-      <c r="DI1" s="7"/>
-      <c r="DJ1" s="7"/>
-      <c r="DK1" s="7"/>
-      <c r="DL1" s="7"/>
-      <c r="DM1" s="7"/>
-      <c r="DN1" s="7"/>
-      <c r="DO1" s="7"/>
-      <c r="DP1" s="7"/>
-      <c r="DQ1" s="7"/>
-      <c r="DR1" s="7"/>
-      <c r="DS1" s="8" t="s">
+      <c r="DC1" s="19"/>
+      <c r="DD1" s="19"/>
+      <c r="DE1" s="19"/>
+      <c r="DF1" s="19"/>
+      <c r="DG1" s="19"/>
+      <c r="DH1" s="19"/>
+      <c r="DI1" s="19"/>
+      <c r="DJ1" s="19"/>
+      <c r="DK1" s="19"/>
+      <c r="DL1" s="19"/>
+      <c r="DM1" s="19"/>
+      <c r="DN1" s="19"/>
+      <c r="DO1" s="19"/>
+      <c r="DP1" s="19"/>
+      <c r="DQ1" s="19"/>
+      <c r="DR1" s="19"/>
+      <c r="DS1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="DT1" s="8"/>
-      <c r="DU1" s="8"/>
-      <c r="DV1" s="8"/>
-      <c r="DW1" s="8"/>
-      <c r="DX1" s="8"/>
-      <c r="DY1" s="8"/>
-      <c r="DZ1" s="8"/>
-      <c r="EA1" s="8"/>
-      <c r="EB1" s="8"/>
-      <c r="EC1" s="8"/>
-      <c r="ED1" s="8"/>
-      <c r="EE1" s="8"/>
-      <c r="EF1" s="8"/>
-      <c r="EG1" s="8"/>
-      <c r="EH1" s="8"/>
-      <c r="EI1" s="8"/>
-      <c r="EJ1" s="8"/>
-      <c r="EK1" s="8"/>
-      <c r="EL1" s="8"/>
-      <c r="EM1" s="8"/>
-      <c r="EN1" s="17" t="s">
+      <c r="DT1" s="18"/>
+      <c r="DU1" s="18"/>
+      <c r="DV1" s="18"/>
+      <c r="DW1" s="18"/>
+      <c r="DX1" s="18"/>
+      <c r="DY1" s="18"/>
+      <c r="DZ1" s="18"/>
+      <c r="EA1" s="18"/>
+      <c r="EB1" s="18"/>
+      <c r="EC1" s="18"/>
+      <c r="ED1" s="18"/>
+      <c r="EE1" s="18"/>
+      <c r="EF1" s="18"/>
+      <c r="EG1" s="18"/>
+      <c r="EH1" s="18"/>
+      <c r="EI1" s="18"/>
+      <c r="EJ1" s="18"/>
+      <c r="EK1" s="18"/>
+      <c r="EL1" s="18"/>
+      <c r="EM1" s="18"/>
+      <c r="EN1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="EO1" s="18"/>
-      <c r="EP1" s="18"/>
-      <c r="EQ1" s="18"/>
-      <c r="ER1" s="18"/>
-      <c r="ES1" s="18"/>
-      <c r="ET1" s="18"/>
-      <c r="EU1" s="19"/>
-      <c r="EV1" s="8" t="s">
+      <c r="EO1" s="10"/>
+      <c r="EP1" s="10"/>
+      <c r="EQ1" s="10"/>
+      <c r="ER1" s="10"/>
+      <c r="ES1" s="10"/>
+      <c r="ET1" s="10"/>
+      <c r="EU1" s="11"/>
+      <c r="EV1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="EW1" s="8"/>
-      <c r="EX1" s="8"/>
-      <c r="EY1" s="8"/>
-      <c r="EZ1" s="8"/>
-      <c r="FA1" s="8"/>
-      <c r="FB1" s="8"/>
-      <c r="FC1" s="8"/>
-      <c r="FD1" s="8"/>
-      <c r="FE1" s="8"/>
-      <c r="FF1" s="8"/>
-      <c r="FG1" s="8"/>
-      <c r="FH1" s="8"/>
-      <c r="FI1" s="8"/>
-      <c r="FJ1" s="8"/>
-      <c r="FK1" s="8"/>
-      <c r="FL1" s="8"/>
-      <c r="FM1" s="8"/>
-      <c r="FN1" s="8"/>
-      <c r="FO1" s="8"/>
-      <c r="FP1" s="8"/>
-      <c r="FQ1" s="8"/>
-      <c r="FR1" s="8"/>
-      <c r="FS1" s="8"/>
-      <c r="FT1" s="8"/>
-      <c r="FU1" s="8"/>
-      <c r="FV1" s="8"/>
-      <c r="FW1" s="8"/>
-      <c r="FX1" s="8"/>
-      <c r="FY1" s="8"/>
-      <c r="FZ1" s="8"/>
-      <c r="GA1" s="8"/>
-      <c r="GB1" s="8"/>
-      <c r="GC1" s="8"/>
-      <c r="GD1" s="8"/>
-      <c r="GE1" s="8"/>
-      <c r="GF1" s="8"/>
-      <c r="GG1" s="8"/>
-      <c r="GH1" s="8"/>
-      <c r="GI1" s="8"/>
-      <c r="GJ1" s="8"/>
-      <c r="GK1" s="8"/>
-      <c r="GL1" s="8"/>
-      <c r="GM1" s="8"/>
-      <c r="GN1" s="8"/>
-      <c r="GO1" s="8"/>
-      <c r="GP1" s="8"/>
-      <c r="GQ1" s="8"/>
-      <c r="GR1" s="8"/>
-      <c r="GS1" s="8"/>
-      <c r="GT1" s="8"/>
-      <c r="GU1" s="8"/>
-      <c r="GV1" s="8"/>
-      <c r="GW1" s="8"/>
+      <c r="EW1" s="18"/>
+      <c r="EX1" s="18"/>
+      <c r="EY1" s="18"/>
+      <c r="EZ1" s="18"/>
+      <c r="FA1" s="18"/>
+      <c r="FB1" s="18"/>
+      <c r="FC1" s="18"/>
+      <c r="FD1" s="18"/>
+      <c r="FE1" s="18"/>
+      <c r="FF1" s="18"/>
+      <c r="FG1" s="18"/>
+      <c r="FH1" s="18"/>
+      <c r="FI1" s="18"/>
+      <c r="FJ1" s="18"/>
+      <c r="FK1" s="18"/>
+      <c r="FL1" s="18"/>
+      <c r="FM1" s="18"/>
+      <c r="FN1" s="18"/>
+      <c r="FO1" s="18"/>
+      <c r="FP1" s="18"/>
+      <c r="FQ1" s="18"/>
+      <c r="FR1" s="18"/>
+      <c r="FS1" s="18"/>
+      <c r="FT1" s="18"/>
+      <c r="FU1" s="18"/>
+      <c r="FV1" s="18"/>
+      <c r="FW1" s="18"/>
+      <c r="FX1" s="18"/>
+      <c r="FY1" s="18"/>
+      <c r="FZ1" s="18"/>
+      <c r="GA1" s="18"/>
+      <c r="GB1" s="18"/>
+      <c r="GC1" s="18"/>
+      <c r="GD1" s="18"/>
+      <c r="GE1" s="18"/>
+      <c r="GF1" s="18"/>
+      <c r="GG1" s="18"/>
+      <c r="GH1" s="18"/>
+      <c r="GI1" s="18"/>
+      <c r="GJ1" s="18"/>
+      <c r="GK1" s="18"/>
+      <c r="GL1" s="18"/>
+      <c r="GM1" s="18"/>
+      <c r="GN1" s="18"/>
+      <c r="GO1" s="18"/>
+      <c r="GP1" s="18"/>
+      <c r="GQ1" s="18"/>
+      <c r="GR1" s="18"/>
+      <c r="GS1" s="18"/>
+      <c r="GT1" s="18"/>
+      <c r="GU1" s="18"/>
+      <c r="GV1" s="18"/>
+      <c r="GW1" s="18"/>
     </row>
     <row r="2" spans="1:205">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
       <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="14" t="s">
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="14" t="s">
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="17"/>
       <c r="AB2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AC2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13" t="s">
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="13" t="s">
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AL2" s="13"/>
-      <c r="AM2" s="13"/>
-      <c r="AN2" s="13"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
       <c r="AO2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AP2" s="13" t="s">
+      <c r="AP2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="13"/>
-      <c r="AR2" s="13"/>
-      <c r="AS2" s="13"/>
-      <c r="AT2" s="13" t="s">
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="13"/>
-      <c r="AV2" s="13"/>
-      <c r="AW2" s="13"/>
-      <c r="AX2" s="13" t="s">
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AY2" s="13"/>
-      <c r="AZ2" s="13"/>
-      <c r="BA2" s="13"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
       <c r="BB2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="BC2" s="13" t="s">
+      <c r="BC2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="BD2" s="13"/>
-      <c r="BE2" s="13"/>
-      <c r="BF2" s="13"/>
-      <c r="BG2" s="13" t="s">
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="BH2" s="13"/>
-      <c r="BI2" s="13"/>
-      <c r="BJ2" s="13"/>
-      <c r="BK2" s="13" t="s">
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="BL2" s="13"/>
-      <c r="BM2" s="13"/>
-      <c r="BN2" s="13"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
+      <c r="BN2" s="8"/>
       <c r="BO2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BP2" s="13" t="s">
+      <c r="BP2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="BQ2" s="13"/>
-      <c r="BR2" s="13"/>
-      <c r="BS2" s="13"/>
-      <c r="BT2" s="13" t="s">
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="BU2" s="13"/>
-      <c r="BV2" s="13"/>
-      <c r="BW2" s="13"/>
-      <c r="BX2" s="13" t="s">
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="BY2" s="13"/>
-      <c r="BZ2" s="13"/>
-      <c r="CA2" s="13"/>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="8"/>
       <c r="CB2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="CC2" s="13" t="s">
+      <c r="CC2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="CD2" s="13"/>
-      <c r="CE2" s="13"/>
-      <c r="CF2" s="13"/>
-      <c r="CG2" s="13" t="s">
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="8"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="CH2" s="13"/>
-      <c r="CI2" s="13"/>
-      <c r="CJ2" s="13"/>
-      <c r="CK2" s="13" t="s">
+      <c r="CH2" s="8"/>
+      <c r="CI2" s="8"/>
+      <c r="CJ2" s="8"/>
+      <c r="CK2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="CL2" s="13"/>
-      <c r="CM2" s="13"/>
-      <c r="CN2" s="13"/>
-      <c r="CO2" s="13" t="s">
+      <c r="CL2" s="8"/>
+      <c r="CM2" s="8"/>
+      <c r="CN2" s="8"/>
+      <c r="CO2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="CP2" s="13"/>
-      <c r="CQ2" s="13"/>
-      <c r="CR2" s="13"/>
-      <c r="CS2" s="13" t="s">
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="8"/>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="CT2" s="13"/>
-      <c r="CU2" s="13"/>
-      <c r="CV2" s="13"/>
-      <c r="CW2" s="13" t="s">
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="CX2" s="13"/>
-      <c r="CY2" s="13"/>
-      <c r="CZ2" s="13"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
+      <c r="CZ2" s="8"/>
       <c r="DA2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="DB2" s="13" t="s">
+      <c r="DB2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="DC2" s="13"/>
-      <c r="DD2" s="13"/>
-      <c r="DE2" s="13"/>
-      <c r="DF2" s="13" t="s">
+      <c r="DC2" s="8"/>
+      <c r="DD2" s="8"/>
+      <c r="DE2" s="8"/>
+      <c r="DF2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="DG2" s="13"/>
-      <c r="DH2" s="13"/>
-      <c r="DI2" s="13"/>
-      <c r="DJ2" s="13" t="s">
+      <c r="DG2" s="8"/>
+      <c r="DH2" s="8"/>
+      <c r="DI2" s="8"/>
+      <c r="DJ2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="DK2" s="13"/>
-      <c r="DL2" s="13"/>
-      <c r="DM2" s="13"/>
-      <c r="DN2" s="13" t="s">
+      <c r="DK2" s="8"/>
+      <c r="DL2" s="8"/>
+      <c r="DM2" s="8"/>
+      <c r="DN2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="DO2" s="13"/>
-      <c r="DP2" s="13"/>
-      <c r="DQ2" s="13"/>
+      <c r="DO2" s="8"/>
+      <c r="DP2" s="8"/>
+      <c r="DQ2" s="8"/>
       <c r="DR2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="DS2" s="13" t="s">
+      <c r="DS2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="DT2" s="13"/>
-      <c r="DU2" s="13"/>
-      <c r="DV2" s="13"/>
-      <c r="DW2" s="13" t="s">
+      <c r="DT2" s="8"/>
+      <c r="DU2" s="8"/>
+      <c r="DV2" s="8"/>
+      <c r="DW2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="DX2" s="13"/>
-      <c r="DY2" s="13"/>
-      <c r="DZ2" s="13"/>
-      <c r="EA2" s="13" t="s">
+      <c r="DX2" s="8"/>
+      <c r="DY2" s="8"/>
+      <c r="DZ2" s="8"/>
+      <c r="EA2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="EB2" s="13"/>
-      <c r="EC2" s="13"/>
-      <c r="ED2" s="13"/>
-      <c r="EE2" s="13" t="s">
+      <c r="EB2" s="8"/>
+      <c r="EC2" s="8"/>
+      <c r="ED2" s="8"/>
+      <c r="EE2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="EF2" s="13"/>
-      <c r="EG2" s="13"/>
-      <c r="EH2" s="13"/>
-      <c r="EI2" s="13" t="s">
+      <c r="EF2" s="8"/>
+      <c r="EG2" s="8"/>
+      <c r="EH2" s="8"/>
+      <c r="EI2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="EJ2" s="13"/>
-      <c r="EK2" s="13"/>
-      <c r="EL2" s="13"/>
+      <c r="EJ2" s="8"/>
+      <c r="EK2" s="8"/>
+      <c r="EL2" s="8"/>
       <c r="EM2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="EN2" s="20"/>
-      <c r="EO2" s="21"/>
-      <c r="EP2" s="21"/>
-      <c r="EQ2" s="21"/>
-      <c r="ER2" s="21"/>
-      <c r="ES2" s="21"/>
-      <c r="ET2" s="21"/>
-      <c r="EU2" s="22"/>
-      <c r="EV2" s="13" t="s">
+      <c r="EN2" s="12"/>
+      <c r="EO2" s="13"/>
+      <c r="EP2" s="13"/>
+      <c r="EQ2" s="13"/>
+      <c r="ER2" s="13"/>
+      <c r="ES2" s="13"/>
+      <c r="ET2" s="13"/>
+      <c r="EU2" s="14"/>
+      <c r="EV2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="EW2" s="13"/>
-      <c r="EX2" s="13"/>
-      <c r="EY2" s="13"/>
-      <c r="EZ2" s="13" t="s">
+      <c r="EW2" s="8"/>
+      <c r="EX2" s="8"/>
+      <c r="EY2" s="8"/>
+      <c r="EZ2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="FA2" s="13"/>
-      <c r="FB2" s="13"/>
-      <c r="FC2" s="13"/>
-      <c r="FD2" s="13" t="s">
+      <c r="FA2" s="8"/>
+      <c r="FB2" s="8"/>
+      <c r="FC2" s="8"/>
+      <c r="FD2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="FE2" s="13"/>
-      <c r="FF2" s="13"/>
-      <c r="FG2" s="13"/>
-      <c r="FH2" s="13" t="s">
+      <c r="FE2" s="8"/>
+      <c r="FF2" s="8"/>
+      <c r="FG2" s="8"/>
+      <c r="FH2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="FI2" s="13"/>
-      <c r="FJ2" s="13"/>
-      <c r="FK2" s="13"/>
-      <c r="FL2" s="13" t="s">
+      <c r="FI2" s="8"/>
+      <c r="FJ2" s="8"/>
+      <c r="FK2" s="8"/>
+      <c r="FL2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="FM2" s="13"/>
-      <c r="FN2" s="13"/>
-      <c r="FO2" s="13"/>
-      <c r="FP2" s="13" t="s">
+      <c r="FM2" s="8"/>
+      <c r="FN2" s="8"/>
+      <c r="FO2" s="8"/>
+      <c r="FP2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="FQ2" s="13"/>
-      <c r="FR2" s="13"/>
-      <c r="FS2" s="13"/>
-      <c r="FT2" s="13" t="s">
+      <c r="FQ2" s="8"/>
+      <c r="FR2" s="8"/>
+      <c r="FS2" s="8"/>
+      <c r="FT2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="FU2" s="13"/>
-      <c r="FV2" s="13"/>
-      <c r="FW2" s="13"/>
-      <c r="FX2" s="13" t="s">
+      <c r="FU2" s="8"/>
+      <c r="FV2" s="8"/>
+      <c r="FW2" s="8"/>
+      <c r="FX2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="FY2" s="13"/>
-      <c r="FZ2" s="13"/>
-      <c r="GA2" s="13"/>
-      <c r="GB2" s="13" t="s">
+      <c r="FY2" s="8"/>
+      <c r="FZ2" s="8"/>
+      <c r="GA2" s="8"/>
+      <c r="GB2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="GC2" s="13"/>
-      <c r="GD2" s="13"/>
-      <c r="GE2" s="13"/>
-      <c r="GF2" s="13" t="s">
+      <c r="GC2" s="8"/>
+      <c r="GD2" s="8"/>
+      <c r="GE2" s="8"/>
+      <c r="GF2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="GG2" s="13"/>
-      <c r="GH2" s="13"/>
-      <c r="GI2" s="13"/>
-      <c r="GJ2" s="13" t="s">
+      <c r="GG2" s="8"/>
+      <c r="GH2" s="8"/>
+      <c r="GI2" s="8"/>
+      <c r="GJ2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="GK2" s="13"/>
-      <c r="GL2" s="13"/>
-      <c r="GM2" s="13"/>
-      <c r="GN2" s="13" t="s">
+      <c r="GK2" s="8"/>
+      <c r="GL2" s="8"/>
+      <c r="GM2" s="8"/>
+      <c r="GN2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="GO2" s="13"/>
-      <c r="GP2" s="13"/>
-      <c r="GQ2" s="13"/>
-      <c r="GR2" s="13" t="s">
+      <c r="GO2" s="8"/>
+      <c r="GP2" s="8"/>
+      <c r="GQ2" s="8"/>
+      <c r="GR2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="GS2" s="13" t="s">
+      <c r="GS2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="GT2" s="13" t="s">
+      <c r="GT2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="GU2" s="13" t="s">
+      <c r="GU2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="GV2" s="13" t="s">
+      <c r="GV2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="GW2" s="13" t="s">
+      <c r="GW2" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1438,10 +1442,10 @@
         <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>46</v>
@@ -1869,8 +1873,8 @@
       <c r="EQ3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="ER3" s="23" t="s">
-        <v>58</v>
+      <c r="ER3" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="ES3" s="2" t="s">
         <v>54</v>
@@ -2025,51 +2029,26 @@
       <c r="GQ3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="GR3" s="13"/>
-      <c r="GS3" s="13"/>
-      <c r="GT3" s="13"/>
-      <c r="GU3" s="13"/>
-      <c r="GV3" s="13"/>
-      <c r="GW3" s="13"/>
+      <c r="GR3" s="8"/>
+      <c r="GS3" s="8"/>
+      <c r="GT3" s="8"/>
+      <c r="GU3" s="8"/>
+      <c r="GV3" s="8"/>
+      <c r="GW3" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="GV2:GV3"/>
-    <mergeCell ref="GW2:GW3"/>
-    <mergeCell ref="GB2:GE2"/>
-    <mergeCell ref="GF2:GI2"/>
-    <mergeCell ref="GJ2:GM2"/>
-    <mergeCell ref="GN2:GQ2"/>
-    <mergeCell ref="GR2:GR3"/>
-    <mergeCell ref="GS2:GS3"/>
-    <mergeCell ref="FL2:FO2"/>
-    <mergeCell ref="FP2:FS2"/>
-    <mergeCell ref="FT2:FW2"/>
-    <mergeCell ref="GT2:GT3"/>
-    <mergeCell ref="GU2:GU3"/>
-    <mergeCell ref="EI2:EL2"/>
-    <mergeCell ref="EV2:EY2"/>
-    <mergeCell ref="EZ2:FC2"/>
-    <mergeCell ref="FD2:FG2"/>
-    <mergeCell ref="FH2:FK2"/>
-    <mergeCell ref="EN1:EU2"/>
-    <mergeCell ref="BX2:CA2"/>
-    <mergeCell ref="CC2:CF2"/>
-    <mergeCell ref="CG2:CJ2"/>
-    <mergeCell ref="CK2:CN2"/>
-    <mergeCell ref="CO2:CR2"/>
-    <mergeCell ref="BT2:BW2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="AK2:AN2"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="AT2:AW2"/>
-    <mergeCell ref="AX2:BA2"/>
-    <mergeCell ref="BC2:BF2"/>
-    <mergeCell ref="BG2:BJ2"/>
-    <mergeCell ref="BK2:BN2"/>
-    <mergeCell ref="BP2:BS2"/>
+    <mergeCell ref="BP1:CB1"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="AC1:AO1"/>
+    <mergeCell ref="AP1:BB1"/>
+    <mergeCell ref="BC1:BO1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:W2"/>
     <mergeCell ref="CC1:DA1"/>
     <mergeCell ref="DB1:DR1"/>
     <mergeCell ref="DS1:EM1"/>
@@ -2085,17 +2064,42 @@
     <mergeCell ref="DW2:DZ2"/>
     <mergeCell ref="EA2:ED2"/>
     <mergeCell ref="EE2:EH2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="BP1:CB1"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AA1"/>
-    <mergeCell ref="AC1:AO1"/>
-    <mergeCell ref="AP1:BB1"/>
-    <mergeCell ref="BC1:BO1"/>
+    <mergeCell ref="BT2:BW2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AG2:AJ2"/>
+    <mergeCell ref="AK2:AN2"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="AT2:AW2"/>
+    <mergeCell ref="AX2:BA2"/>
+    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="BG2:BJ2"/>
+    <mergeCell ref="BK2:BN2"/>
+    <mergeCell ref="BP2:BS2"/>
+    <mergeCell ref="BX2:CA2"/>
+    <mergeCell ref="CC2:CF2"/>
+    <mergeCell ref="CG2:CJ2"/>
+    <mergeCell ref="CK2:CN2"/>
+    <mergeCell ref="CO2:CR2"/>
+    <mergeCell ref="EI2:EL2"/>
+    <mergeCell ref="EV2:EY2"/>
+    <mergeCell ref="EZ2:FC2"/>
+    <mergeCell ref="FD2:FG2"/>
+    <mergeCell ref="FH2:FK2"/>
+    <mergeCell ref="EN1:EU2"/>
+    <mergeCell ref="FL2:FO2"/>
+    <mergeCell ref="FP2:FS2"/>
+    <mergeCell ref="FT2:FW2"/>
+    <mergeCell ref="GT2:GT3"/>
+    <mergeCell ref="GU2:GU3"/>
+    <mergeCell ref="GV2:GV3"/>
+    <mergeCell ref="GW2:GW3"/>
+    <mergeCell ref="GB2:GE2"/>
+    <mergeCell ref="GF2:GI2"/>
+    <mergeCell ref="GJ2:GM2"/>
+    <mergeCell ref="GN2:GQ2"/>
+    <mergeCell ref="GR2:GR3"/>
+    <mergeCell ref="GS2:GS3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
DEBUG: wadd hp and line item to ppp xlsx from the upload button in menu. Add team grade in shotchart xlsx
</commit_message>
<xml_diff>
--- a/basketBallRecorder/PPP數據.xlsx
+++ b/basketBallRecorder/PPP數據.xlsx
@@ -555,6 +555,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,45 +606,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,9 +622,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1023,178 +1023,178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HR3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="EG1" workbookViewId="0">
+      <selection activeCell="EP15" sqref="EP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="204" width="10.83203125" customWidth="1"/>
+    <col min="2" max="226" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:226">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
       <c r="O1" s="21"/>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
       <c r="AB1" s="1"/>
-      <c r="AC1" s="19" t="s">
+      <c r="AC1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="20" t="s">
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="20"/>
+      <c r="AN1" s="20"/>
+      <c r="AO1" s="20"/>
+      <c r="AP1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20"/>
-      <c r="BC1" s="24" t="s">
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="24"/>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
-      <c r="BJ1" s="24"/>
-      <c r="BK1" s="24"/>
-      <c r="BL1" s="24"/>
-      <c r="BM1" s="24"/>
-      <c r="BN1" s="24"/>
-      <c r="BO1" s="24"/>
-      <c r="BP1" s="20" t="s">
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BQ1" s="20"/>
-      <c r="BR1" s="20"/>
-      <c r="BS1" s="20"/>
-      <c r="BT1" s="20"/>
-      <c r="BU1" s="20"/>
-      <c r="BV1" s="20"/>
-      <c r="BW1" s="20"/>
-      <c r="BX1" s="20"/>
-      <c r="BY1" s="20"/>
-      <c r="BZ1" s="20"/>
-      <c r="CA1" s="20"/>
-      <c r="CB1" s="20"/>
-      <c r="CC1" s="19" t="s">
+      <c r="BQ1" s="19"/>
+      <c r="BR1" s="19"/>
+      <c r="BS1" s="19"/>
+      <c r="BT1" s="19"/>
+      <c r="BU1" s="19"/>
+      <c r="BV1" s="19"/>
+      <c r="BW1" s="19"/>
+      <c r="BX1" s="19"/>
+      <c r="BY1" s="19"/>
+      <c r="BZ1" s="19"/>
+      <c r="CA1" s="19"/>
+      <c r="CB1" s="19"/>
+      <c r="CC1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="CD1" s="19"/>
-      <c r="CE1" s="19"/>
-      <c r="CF1" s="19"/>
-      <c r="CG1" s="19"/>
-      <c r="CH1" s="19"/>
-      <c r="CI1" s="19"/>
-      <c r="CJ1" s="19"/>
-      <c r="CK1" s="19"/>
-      <c r="CL1" s="19"/>
-      <c r="CM1" s="19"/>
-      <c r="CN1" s="19"/>
-      <c r="CO1" s="19"/>
-      <c r="CP1" s="19"/>
-      <c r="CQ1" s="19"/>
-      <c r="CR1" s="19"/>
-      <c r="CS1" s="19"/>
-      <c r="CT1" s="19"/>
-      <c r="CU1" s="19"/>
-      <c r="CV1" s="19"/>
-      <c r="CW1" s="19"/>
-      <c r="CX1" s="19"/>
-      <c r="CY1" s="19"/>
-      <c r="CZ1" s="19"/>
-      <c r="DA1" s="19"/>
-      <c r="DB1" s="20" t="s">
+      <c r="CD1" s="20"/>
+      <c r="CE1" s="20"/>
+      <c r="CF1" s="20"/>
+      <c r="CG1" s="20"/>
+      <c r="CH1" s="20"/>
+      <c r="CI1" s="20"/>
+      <c r="CJ1" s="20"/>
+      <c r="CK1" s="20"/>
+      <c r="CL1" s="20"/>
+      <c r="CM1" s="20"/>
+      <c r="CN1" s="20"/>
+      <c r="CO1" s="20"/>
+      <c r="CP1" s="20"/>
+      <c r="CQ1" s="20"/>
+      <c r="CR1" s="20"/>
+      <c r="CS1" s="20"/>
+      <c r="CT1" s="20"/>
+      <c r="CU1" s="20"/>
+      <c r="CV1" s="20"/>
+      <c r="CW1" s="20"/>
+      <c r="CX1" s="20"/>
+      <c r="CY1" s="20"/>
+      <c r="CZ1" s="20"/>
+      <c r="DA1" s="20"/>
+      <c r="DB1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="DC1" s="20"/>
-      <c r="DD1" s="20"/>
-      <c r="DE1" s="20"/>
-      <c r="DF1" s="20"/>
-      <c r="DG1" s="20"/>
-      <c r="DH1" s="20"/>
-      <c r="DI1" s="20"/>
-      <c r="DJ1" s="20"/>
-      <c r="DK1" s="20"/>
-      <c r="DL1" s="20"/>
-      <c r="DM1" s="20"/>
-      <c r="DN1" s="20"/>
-      <c r="DO1" s="20"/>
-      <c r="DP1" s="20"/>
-      <c r="DQ1" s="20"/>
-      <c r="DR1" s="20"/>
-      <c r="DS1" s="19" t="s">
+      <c r="DC1" s="19"/>
+      <c r="DD1" s="19"/>
+      <c r="DE1" s="19"/>
+      <c r="DF1" s="19"/>
+      <c r="DG1" s="19"/>
+      <c r="DH1" s="19"/>
+      <c r="DI1" s="19"/>
+      <c r="DJ1" s="19"/>
+      <c r="DK1" s="19"/>
+      <c r="DL1" s="19"/>
+      <c r="DM1" s="19"/>
+      <c r="DN1" s="19"/>
+      <c r="DO1" s="19"/>
+      <c r="DP1" s="19"/>
+      <c r="DQ1" s="19"/>
+      <c r="DR1" s="19"/>
+      <c r="DS1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="DT1" s="19"/>
-      <c r="DU1" s="19"/>
-      <c r="DV1" s="19"/>
-      <c r="DW1" s="19"/>
-      <c r="DX1" s="19"/>
-      <c r="DY1" s="19"/>
-      <c r="DZ1" s="19"/>
-      <c r="EA1" s="19"/>
-      <c r="EB1" s="19"/>
-      <c r="EC1" s="19"/>
-      <c r="ED1" s="19"/>
-      <c r="EE1" s="19"/>
-      <c r="EF1" s="19"/>
-      <c r="EG1" s="19"/>
-      <c r="EH1" s="19"/>
-      <c r="EI1" s="19"/>
-      <c r="EJ1" s="19"/>
-      <c r="EK1" s="19"/>
-      <c r="EL1" s="19"/>
-      <c r="EM1" s="19"/>
+      <c r="DT1" s="20"/>
+      <c r="DU1" s="20"/>
+      <c r="DV1" s="20"/>
+      <c r="DW1" s="20"/>
+      <c r="DX1" s="20"/>
+      <c r="DY1" s="20"/>
+      <c r="DZ1" s="20"/>
+      <c r="EA1" s="20"/>
+      <c r="EB1" s="20"/>
+      <c r="EC1" s="20"/>
+      <c r="ED1" s="20"/>
+      <c r="EE1" s="20"/>
+      <c r="EF1" s="20"/>
+      <c r="EG1" s="20"/>
+      <c r="EH1" s="20"/>
+      <c r="EI1" s="20"/>
+      <c r="EJ1" s="20"/>
+      <c r="EK1" s="20"/>
+      <c r="EL1" s="20"/>
+      <c r="EM1" s="20"/>
       <c r="EN1" s="16" t="s">
         <v>59</v>
       </c>
@@ -1214,76 +1214,76 @@
       <c r="FB1" s="17"/>
       <c r="FC1" s="17"/>
       <c r="FD1" s="18"/>
-      <c r="FE1" s="25" t="s">
+      <c r="FE1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="FF1" s="26"/>
-      <c r="FG1" s="26"/>
-      <c r="FH1" s="26"/>
-      <c r="FI1" s="26"/>
-      <c r="FJ1" s="26"/>
-      <c r="FK1" s="26"/>
-      <c r="FL1" s="27"/>
-      <c r="FM1" s="22" t="s">
+      <c r="FF1" s="27"/>
+      <c r="FG1" s="27"/>
+      <c r="FH1" s="27"/>
+      <c r="FI1" s="27"/>
+      <c r="FJ1" s="27"/>
+      <c r="FK1" s="27"/>
+      <c r="FL1" s="28"/>
+      <c r="FM1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="FN1" s="23"/>
-      <c r="FO1" s="23"/>
-      <c r="FP1" s="23"/>
-      <c r="FQ1" s="23"/>
-      <c r="FR1" s="23"/>
-      <c r="FS1" s="23"/>
-      <c r="FT1" s="23"/>
-      <c r="FU1" s="23"/>
-      <c r="FV1" s="23"/>
-      <c r="FW1" s="23"/>
-      <c r="FX1" s="23"/>
-      <c r="FY1" s="23"/>
-      <c r="FZ1" s="23"/>
-      <c r="GA1" s="23"/>
-      <c r="GB1" s="23"/>
-      <c r="GC1" s="23"/>
-      <c r="GD1" s="23"/>
-      <c r="GE1" s="23"/>
-      <c r="GF1" s="23"/>
-      <c r="GG1" s="23"/>
-      <c r="GH1" s="23"/>
-      <c r="GI1" s="23"/>
-      <c r="GJ1" s="23"/>
-      <c r="GK1" s="23"/>
-      <c r="GL1" s="23"/>
-      <c r="GM1" s="23"/>
-      <c r="GN1" s="23"/>
-      <c r="GO1" s="23"/>
-      <c r="GP1" s="23"/>
-      <c r="GQ1" s="23"/>
-      <c r="GR1" s="23"/>
-      <c r="GS1" s="23"/>
-      <c r="GT1" s="23"/>
-      <c r="GU1" s="23"/>
-      <c r="GV1" s="23"/>
-      <c r="GW1" s="23"/>
-      <c r="GX1" s="23"/>
-      <c r="GY1" s="23"/>
-      <c r="GZ1" s="23"/>
-      <c r="HA1" s="23"/>
-      <c r="HB1" s="23"/>
-      <c r="HC1" s="23"/>
-      <c r="HD1" s="23"/>
-      <c r="HE1" s="23"/>
-      <c r="HF1" s="23"/>
-      <c r="HG1" s="23"/>
-      <c r="HH1" s="23"/>
-      <c r="HI1" s="23"/>
-      <c r="HJ1" s="23"/>
-      <c r="HK1" s="23"/>
-      <c r="HL1" s="23"/>
-      <c r="HM1" s="23"/>
-      <c r="HN1" s="23"/>
-      <c r="HO1" s="23"/>
-      <c r="HP1" s="23"/>
-      <c r="HQ1" s="23"/>
-      <c r="HR1" s="31"/>
+      <c r="FN1" s="14"/>
+      <c r="FO1" s="14"/>
+      <c r="FP1" s="14"/>
+      <c r="FQ1" s="14"/>
+      <c r="FR1" s="14"/>
+      <c r="FS1" s="14"/>
+      <c r="FT1" s="14"/>
+      <c r="FU1" s="14"/>
+      <c r="FV1" s="14"/>
+      <c r="FW1" s="14"/>
+      <c r="FX1" s="14"/>
+      <c r="FY1" s="14"/>
+      <c r="FZ1" s="14"/>
+      <c r="GA1" s="14"/>
+      <c r="GB1" s="14"/>
+      <c r="GC1" s="14"/>
+      <c r="GD1" s="14"/>
+      <c r="GE1" s="14"/>
+      <c r="GF1" s="14"/>
+      <c r="GG1" s="14"/>
+      <c r="GH1" s="14"/>
+      <c r="GI1" s="14"/>
+      <c r="GJ1" s="14"/>
+      <c r="GK1" s="14"/>
+      <c r="GL1" s="14"/>
+      <c r="GM1" s="14"/>
+      <c r="GN1" s="14"/>
+      <c r="GO1" s="14"/>
+      <c r="GP1" s="14"/>
+      <c r="GQ1" s="14"/>
+      <c r="GR1" s="14"/>
+      <c r="GS1" s="14"/>
+      <c r="GT1" s="14"/>
+      <c r="GU1" s="14"/>
+      <c r="GV1" s="14"/>
+      <c r="GW1" s="14"/>
+      <c r="GX1" s="14"/>
+      <c r="GY1" s="14"/>
+      <c r="GZ1" s="14"/>
+      <c r="HA1" s="14"/>
+      <c r="HB1" s="14"/>
+      <c r="HC1" s="14"/>
+      <c r="HD1" s="14"/>
+      <c r="HE1" s="14"/>
+      <c r="HF1" s="14"/>
+      <c r="HG1" s="14"/>
+      <c r="HH1" s="14"/>
+      <c r="HI1" s="14"/>
+      <c r="HJ1" s="14"/>
+      <c r="HK1" s="14"/>
+      <c r="HL1" s="14"/>
+      <c r="HM1" s="14"/>
+      <c r="HN1" s="14"/>
+      <c r="HO1" s="14"/>
+      <c r="HP1" s="14"/>
+      <c r="HQ1" s="14"/>
+      <c r="HR1" s="15"/>
     </row>
     <row r="2" spans="1:226">
       <c r="A2" s="7"/>
@@ -1309,24 +1309,24 @@
       <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="11"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="25"/>
       <c r="T2" s="16" t="s">
         <v>13</v>
       </c>
       <c r="U2" s="17"/>
       <c r="V2" s="17"/>
       <c r="W2" s="18"/>
-      <c r="X2" s="9" t="s">
+      <c r="X2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="11"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="25"/>
       <c r="AB2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1342,12 +1342,12 @@
       <c r="AH2" s="17"/>
       <c r="AI2" s="17"/>
       <c r="AJ2" s="18"/>
-      <c r="AK2" s="13" t="s">
+      <c r="AK2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="15"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="11"/>
       <c r="AO2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1363,12 +1363,12 @@
       <c r="AU2" s="17"/>
       <c r="AV2" s="17"/>
       <c r="AW2" s="18"/>
-      <c r="AX2" s="13" t="s">
+      <c r="AX2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AY2" s="14"/>
-      <c r="AZ2" s="14"/>
-      <c r="BA2" s="15"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="11"/>
       <c r="BB2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1384,12 +1384,12 @@
       <c r="BH2" s="17"/>
       <c r="BI2" s="17"/>
       <c r="BJ2" s="18"/>
-      <c r="BK2" s="13" t="s">
+      <c r="BK2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="BL2" s="14"/>
-      <c r="BM2" s="14"/>
-      <c r="BN2" s="15"/>
+      <c r="BL2" s="10"/>
+      <c r="BM2" s="10"/>
+      <c r="BN2" s="11"/>
       <c r="BO2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1405,12 +1405,12 @@
       <c r="BU2" s="17"/>
       <c r="BV2" s="17"/>
       <c r="BW2" s="18"/>
-      <c r="BX2" s="13" t="s">
+      <c r="BX2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="BY2" s="14"/>
-      <c r="BZ2" s="14"/>
-      <c r="CA2" s="15"/>
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="11"/>
       <c r="CB2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1465,12 +1465,12 @@
       <c r="DG2" s="17"/>
       <c r="DH2" s="17"/>
       <c r="DI2" s="18"/>
-      <c r="DJ2" s="13" t="s">
+      <c r="DJ2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="DK2" s="14"/>
-      <c r="DL2" s="14"/>
-      <c r="DM2" s="15"/>
+      <c r="DK2" s="10"/>
+      <c r="DL2" s="10"/>
+      <c r="DM2" s="11"/>
       <c r="DN2" s="12" t="s">
         <v>25</v>
       </c>
@@ -1492,12 +1492,12 @@
       <c r="DX2" s="17"/>
       <c r="DY2" s="17"/>
       <c r="DZ2" s="18"/>
-      <c r="EA2" s="13" t="s">
+      <c r="EA2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="EB2" s="14"/>
-      <c r="EC2" s="14"/>
-      <c r="ED2" s="15"/>
+      <c r="EB2" s="10"/>
+      <c r="EC2" s="10"/>
+      <c r="ED2" s="11"/>
       <c r="EE2" s="12" t="s">
         <v>27</v>
       </c>
@@ -1525,12 +1525,12 @@
       <c r="ES2" s="17"/>
       <c r="ET2" s="17"/>
       <c r="EU2" s="18"/>
-      <c r="EV2" s="13" t="s">
+      <c r="EV2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="EW2" s="14"/>
-      <c r="EX2" s="14"/>
-      <c r="EY2" s="15"/>
+      <c r="EW2" s="10"/>
+      <c r="EX2" s="10"/>
+      <c r="EY2" s="11"/>
       <c r="EZ2" s="12" t="s">
         <v>60</v>
       </c>
@@ -1540,14 +1540,14 @@
       <c r="FD2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="FE2" s="28"/>
-      <c r="FF2" s="29"/>
-      <c r="FG2" s="29"/>
-      <c r="FH2" s="29"/>
-      <c r="FI2" s="29"/>
-      <c r="FJ2" s="29"/>
-      <c r="FK2" s="29"/>
-      <c r="FL2" s="30"/>
+      <c r="FE2" s="29"/>
+      <c r="FF2" s="30"/>
+      <c r="FG2" s="30"/>
+      <c r="FH2" s="30"/>
+      <c r="FI2" s="30"/>
+      <c r="FJ2" s="30"/>
+      <c r="FK2" s="30"/>
+      <c r="FL2" s="31"/>
       <c r="FM2" s="12" t="s">
         <v>11</v>
       </c>
@@ -2315,58 +2315,6 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="EV2:EY2"/>
-    <mergeCell ref="GG2:GJ2"/>
-    <mergeCell ref="FM1:HR1"/>
-    <mergeCell ref="EN1:FD1"/>
-    <mergeCell ref="EN2:EQ2"/>
-    <mergeCell ref="ER2:EU2"/>
-    <mergeCell ref="EZ2:FC2"/>
-    <mergeCell ref="BP1:CB1"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AA1"/>
-    <mergeCell ref="AC1:AO1"/>
-    <mergeCell ref="AP1:BB1"/>
-    <mergeCell ref="BC1:BO1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="DF2:DI2"/>
-    <mergeCell ref="DJ2:DM2"/>
-    <mergeCell ref="DN2:DQ2"/>
-    <mergeCell ref="GS2:GV2"/>
-    <mergeCell ref="DW2:DZ2"/>
-    <mergeCell ref="EA2:ED2"/>
-    <mergeCell ref="EE2:EH2"/>
-    <mergeCell ref="EI2:EL2"/>
-    <mergeCell ref="BT2:BW2"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="AK2:AN2"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="AT2:AW2"/>
-    <mergeCell ref="AX2:BA2"/>
-    <mergeCell ref="BC2:BF2"/>
-    <mergeCell ref="BG2:BJ2"/>
-    <mergeCell ref="BK2:BN2"/>
-    <mergeCell ref="BP2:BS2"/>
-    <mergeCell ref="FQ2:FT2"/>
-    <mergeCell ref="FY2:GB2"/>
-    <mergeCell ref="FE1:FL2"/>
-    <mergeCell ref="BX2:CA2"/>
-    <mergeCell ref="CC2:CF2"/>
-    <mergeCell ref="CG2:CJ2"/>
-    <mergeCell ref="CK2:CN2"/>
-    <mergeCell ref="CO2:CR2"/>
-    <mergeCell ref="CC1:DA1"/>
-    <mergeCell ref="DB1:DR1"/>
-    <mergeCell ref="DS1:EM1"/>
-    <mergeCell ref="DS2:DV2"/>
-    <mergeCell ref="CS2:CV2"/>
-    <mergeCell ref="CW2:CZ2"/>
-    <mergeCell ref="DB2:DE2"/>
     <mergeCell ref="X2:AA2"/>
     <mergeCell ref="FU2:FX2"/>
     <mergeCell ref="HQ2:HQ3"/>
@@ -2383,6 +2331,58 @@
     <mergeCell ref="HO2:HO3"/>
     <mergeCell ref="HP2:HP3"/>
     <mergeCell ref="FM2:FP2"/>
+    <mergeCell ref="CC1:DA1"/>
+    <mergeCell ref="DB1:DR1"/>
+    <mergeCell ref="DS1:EM1"/>
+    <mergeCell ref="DS2:DV2"/>
+    <mergeCell ref="CS2:CV2"/>
+    <mergeCell ref="CW2:CZ2"/>
+    <mergeCell ref="DB2:DE2"/>
+    <mergeCell ref="BX2:CA2"/>
+    <mergeCell ref="CC2:CF2"/>
+    <mergeCell ref="CG2:CJ2"/>
+    <mergeCell ref="CK2:CN2"/>
+    <mergeCell ref="CO2:CR2"/>
+    <mergeCell ref="BT2:BW2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AG2:AJ2"/>
+    <mergeCell ref="AK2:AN2"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="AT2:AW2"/>
+    <mergeCell ref="AX2:BA2"/>
+    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="BG2:BJ2"/>
+    <mergeCell ref="BK2:BN2"/>
+    <mergeCell ref="BP2:BS2"/>
+    <mergeCell ref="DF2:DI2"/>
+    <mergeCell ref="DJ2:DM2"/>
+    <mergeCell ref="DN2:DQ2"/>
+    <mergeCell ref="GS2:GV2"/>
+    <mergeCell ref="DW2:DZ2"/>
+    <mergeCell ref="EA2:ED2"/>
+    <mergeCell ref="EE2:EH2"/>
+    <mergeCell ref="EI2:EL2"/>
+    <mergeCell ref="FQ2:FT2"/>
+    <mergeCell ref="FY2:GB2"/>
+    <mergeCell ref="FE1:FL2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="BP1:CB1"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="AC1:AO1"/>
+    <mergeCell ref="AP1:BB1"/>
+    <mergeCell ref="BC1:BO1"/>
+    <mergeCell ref="EV2:EY2"/>
+    <mergeCell ref="GG2:GJ2"/>
+    <mergeCell ref="FM1:HR1"/>
+    <mergeCell ref="EN1:FD1"/>
+    <mergeCell ref="EN2:EQ2"/>
+    <mergeCell ref="ER2:EU2"/>
+    <mergeCell ref="EZ2:FC2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>